<commit_message>
[bug] For bug 50447: rename default color scheme "Office" -> "New Office"
</commit_message>
<xml_diff>
--- a/new/bg-BG/new.xlsx
+++ b/new/bg-BG/new.xlsx
@@ -72,7 +72,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="New Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -112,7 +112,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>

</xml_diff>